<commit_message>
add plot for only present
</commit_message>
<xml_diff>
--- a/data/kpi_example_c02.xlsx
+++ b/data/kpi_example_c02.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CCE976-2521-4E47-8C8F-470155D6DC75}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC98CFD-5A7E-4341-8B58-653F90A04409}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="present" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>scenarios</t>
   </si>
@@ -368,8 +370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,4 +555,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347AC872-03E4-4C6D-99C3-6E0B1D3A16FE}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2015</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>